<commit_message>
Template updated with MSM data and minor changes
fixed template to include MSM data and rel_inc etc.
loaded some additional datapoints into loaddata and added them as global vars to testing
minor changes to testing to get the calibration working - there were some vars defined after the calibration that were needed for the calibration
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -4,28 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12345" tabRatio="768" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="20730" windowHeight="11760" tabRatio="923" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
     <sheet name="cases" sheetId="5" r:id="rId2"/>
     <sheet name="diagnoses" sheetId="12" r:id="rId3"/>
     <sheet name="disease" sheetId="4" r:id="rId4"/>
-    <sheet name="disease_HIV" sheetId="20" r:id="rId5"/>
+    <sheet name="disease_HIV" sheetId="16" r:id="rId5"/>
     <sheet name="cascade_all" sheetId="2" r:id="rId6"/>
     <sheet name="prev_PWID" sheetId="1" r:id="rId7"/>
     <sheet name="cascade_PWID" sheetId="3" r:id="rId8"/>
-    <sheet name="prev_MSM" sheetId="16" r:id="rId9"/>
-    <sheet name="OR HCV by HIV MSM" sheetId="19" r:id="rId10"/>
-    <sheet name="cascade_MSM" sheetId="18" r:id="rId11"/>
-    <sheet name="Interventions_PWID" sheetId="13" r:id="rId12"/>
-    <sheet name="other_epi" sheetId="6" r:id="rId13"/>
-    <sheet name="costs" sheetId="8" r:id="rId14"/>
-    <sheet name="health_utilities" sheetId="9" r:id="rId15"/>
-    <sheet name="transition_rates" sheetId="10" r:id="rId16"/>
-    <sheet name="HCC" sheetId="11" r:id="rId17"/>
-    <sheet name="structure" sheetId="14" r:id="rId18"/>
-    <sheet name="calibration_guess" sheetId="15" r:id="rId19"/>
+    <sheet name="prev_MSM" sheetId="17" r:id="rId9"/>
+    <sheet name="cascade_MSM" sheetId="18" r:id="rId10"/>
+    <sheet name="Interventions_PWID" sheetId="13" r:id="rId11"/>
+    <sheet name="other_epi" sheetId="6" r:id="rId12"/>
+    <sheet name="costs" sheetId="8" r:id="rId13"/>
+    <sheet name="health_utilities" sheetId="9" r:id="rId14"/>
+    <sheet name="transition_rates" sheetId="10" r:id="rId15"/>
+    <sheet name="HCC" sheetId="11" r:id="rId16"/>
+    <sheet name="structure" sheetId="14" r:id="rId17"/>
+    <sheet name="calibration_guess" sheetId="15" r:id="rId18"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -45,7 +44,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nick:</t>
         </r>
@@ -54,7 +53,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Iversen, J., Grebely, J., Catlett, B., Cunningham, P., Dore, G. J., &amp; Maher, L. (2017). Estimating the cascade of hepatitis C testing, care and treatment among people who inject drugs in Australia. International Journal of Drug Policy.</t>
@@ -79,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nick:</t>
         </r>
@@ -88,7 +87,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Dan O'Keefe: 50% of MIX consistenly covered across interviews, 45% inconsistently covered (i.e. cycling) and 5% consistently uncovered. </t>
@@ -103,7 +102,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nick:</t>
         </r>
@@ -112,7 +111,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Stafford, J., &amp; Breen, C. (2015). Australian Drug Trends 2015. Findings from the Illicit Drug Reporting System (IDRS). National Drug and Alcohol Research Centre, University of New South Wales, Sydney, Australia. Australian Drug Trends Series No. 145, ISBN 978-0-7334-3623-9.</t>
@@ -123,8 +122,142 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Nick</author>
+  </authors>
+  <commentList>
+    <comment ref="B39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Burns L, Randall D, Hall W, Law M, Butler T, Bell J, et al. Opioid agonist pharmacotherapy in New SouthWales from 1985 to 2006: patient characteristics and patterns and predictors of treatment retention. Addiction 2009;104:1363–1372.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+29% changed from covered to not covered between annual interviews
+O’Keefe, D., Scott, N., Aitken, C., &amp; Dietze, P. (2017). Longitudinal analysis of change in individual-level needle and syringe coverage amongst a cohort of people who inject drugs in Melbourne, Australia. Drug and Alcohol Dependence, 176, 7-13.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Turner, K. M., Hutchinson, S., Vickerman, P., Hope, V., Craine, N., Palmateer, N., ... &amp; Parry, J. (2011). The impact of needle and syringe provision and opiate substitution therapy on the incidence of hepatitis C virus in injecting drug users: pooling of UK evidence. Addiction, 106(11), 1978-1988.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+35% reduction in injecting frequency for PWID on OST
+Scott, N., Caulkins, J. P., Ritter, A., &amp; Dietze, P. (2015). How patterns of injecting drug use evolve in a cohort of people who inject drugs. Trends and Issues in Crime and Criminal Justice, (502), 1.
+Also 0.41 from:
+Turner, K. M., Hutchinson, S., Vickerman, P., Hope, V., Craine, N., Palmateer, N., ... &amp; Parry, J. (2011). The impact of needle and syringe provision and opiate substitution therapy on the incidence of hepatitis C virus in injecting drug users: pooling of UK evidence. Addiction, 106(11), 1978-1988.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Turner, K. M., Hutchinson, S., Vickerman, P., Hope, V., Craine, N., Palmateer, N., ... &amp; Parry, J. (2011). The impact of needle and syringe provision and opiate substitution therapy on the incidence of hepatitis C virus in injecting drug users: pooling of UK evidence. Addiction, 106(11), 1978-1988.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="282">
   <si>
     <t>Year</t>
   </si>
@@ -672,6 +805,9 @@
     <t>Initial proportion of PWID infected (i.e. 1950)</t>
   </si>
   <si>
+    <t>Proportion of initial model population who are PWID</t>
+  </si>
+  <si>
     <t>Total number of PWID at peak in year 2000</t>
   </si>
   <si>
@@ -933,85 +1069,49 @@
     <t>rel_incidence_NSPOST</t>
   </si>
   <si>
+    <t>r_inc_up</t>
+  </si>
+  <si>
+    <t>Rate ratio of progression (HIV coinfected vs HCV monoinfected)</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>UL</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Thein et al 2008 meta-analysis (approx 70% of patients on HAART)</t>
+  </si>
+  <si>
     <t>HIV status</t>
   </si>
   <si>
-    <t>Prevalence type (anti-HCV or HCV RNA)</t>
-  </si>
-  <si>
-    <t>prevalence</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>positive</t>
-  </si>
-  <si>
-    <t>anti-HCV</t>
+    <t>anti-HCV prevalence</t>
+  </si>
+  <si>
+    <t>estimated HCV RNA prev</t>
   </si>
   <si>
     <t>denominator</t>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>Sentinel surveillance</t>
   </si>
   <si>
-    <t>OR antiHCV HIV-infected vs uninfected</t>
-  </si>
-  <si>
-    <t>Lower bound CI</t>
-  </si>
-  <si>
-    <t>Upper bound CI</t>
-  </si>
-  <si>
-    <t>Platt Systematic review 2016</t>
-  </si>
-  <si>
-    <t>Number of initial model population who are PWID</t>
-  </si>
-  <si>
-    <t>Possibly move this to an Epi sheet?</t>
-  </si>
-  <si>
-    <t>Median year of study 2009</t>
-  </si>
-  <si>
-    <t>negative</t>
+    <t>HCV RNA prevalence estimated using Smith Jordan et al 2016 meta-analysis</t>
   </si>
   <si>
     <t>Sydney Health in Men cohort</t>
-  </si>
-  <si>
-    <t>Initiated treatment</t>
-  </si>
-  <si>
-    <t>Gay periodic Sydney 2011, self-report</t>
-  </si>
-  <si>
-    <t>Rate ratio of progression (HIV coinfected vs HCV monoinfected)</t>
-  </si>
-  <si>
-    <t>RR</t>
-  </si>
-  <si>
-    <t>LL</t>
-  </si>
-  <si>
-    <t>UL</t>
-  </si>
-  <si>
-    <t>Thein et al 2008 meta-analysis (approx 70% of patients on HAART)</t>
-  </si>
-  <si>
-    <t>estimated HCV RNA prev</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>HCV RNA prevalence estimated using Smith Jordan et al 2016 meta-analysis</t>
   </si>
   <si>
     <r>
@@ -1044,7 +1144,13 @@
     <t>Antibody diagnosed</t>
   </si>
   <si>
+    <t>Initiated treatment</t>
+  </si>
+  <si>
     <t>Sentinel surveillance(RNA test % was only measured among those with incident infection so may be overestimated)- antibody diagnosed % is % of all HIV positive MSM with a HCV test so may be underestimate if testing is targeted at high risk</t>
+  </si>
+  <si>
+    <t>Gay periodic Sydney 2011, self-report</t>
   </si>
 </sst>
 </file>
@@ -1099,14 +1205,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1159,7 +1265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1218,11 +1324,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1530,7 +1633,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,106 +1647,35 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>7.5</v>
-      </c>
-      <c r="B2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C2">
-        <v>12.7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="125" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="7" width="11.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
-        <v>288</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-    </row>
-    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -1655,18 +1687,18 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2009</v>
       </c>
-      <c r="B3" t="s">
-        <v>265</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0.73</v>
@@ -1676,35 +1708,35 @@
         <v>0.64575800000000005</v>
       </c>
       <c r="H3" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2011</v>
       </c>
-      <c r="B4" t="s">
-        <v>265</v>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0.86</v>
       </c>
       <c r="H4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2011</v>
       </c>
-      <c r="B5" t="s">
-        <v>276</v>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0.748</v>
       </c>
       <c r="H5" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -1712,7 +1744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -1720,7 +1752,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,15 +1785,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1825,7 @@
         <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1801,10 +1833,10 @@
         <v>146</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D3" s="12"/>
     </row>
@@ -1816,7 +1848,7 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1827,7 +1859,7 @@
         <v>8.3000000000000001E-3</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1839,10 +1871,10 @@
         <v>4.4009682840403613E-4</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1854,7 +1886,7 @@
         <v>6.6021789587945585E-4</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1866,7 +1898,7 @@
         <v>6.6021789587945585E-4</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1878,7 +1910,7 @@
         <v>9.9049037367338576E-4</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,7 +1922,7 @@
         <v>1.6613793266661854E-3</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1902,7 +1934,7 @@
         <v>5.1733587739974654E-3</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1914,7 +1946,7 @@
         <v>1.4240922290342446E-2</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,7 +1958,7 @@
         <v>4.874916500990898E-2</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1938,7 +1970,7 @@
         <v>0.17488924497665875</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1950,10 +1982,10 @@
         <v>9.6463770518054499E-3</v>
       </c>
       <c r="C15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1965,7 +1997,7 @@
         <v>9.6463770518054499E-3</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1977,19 +2009,19 @@
         <v>1.1263192278710714E-2</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B18">
         <f>-LN(1-0.0018)</f>
         <v>1.8016219466282088E-3</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2023,7 +2055,7 @@
         <v>500</v>
       </c>
       <c r="C21" t="s">
-        <v>273</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2034,7 +2066,7 @@
         <v>90000</v>
       </c>
       <c r="C22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2045,7 +2077,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2053,14 +2085,14 @@
         <v>16</v>
       </c>
       <c r="B24" s="17">
-        <f>1/17</f>
-        <v>5.8823529411764705E-2</v>
+        <f>1/14</f>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2072,10 +2104,10 @@
         <v>2.7371196796132015E-2</v>
       </c>
       <c r="C25" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2086,7 +2118,7 @@
         <v>0.6</v>
       </c>
       <c r="C26" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2097,7 +2129,7 @@
         <v>0.9</v>
       </c>
       <c r="C27" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,7 +2140,7 @@
         <v>0.1</v>
       </c>
       <c r="C28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2119,7 +2151,7 @@
         <v>0.9</v>
       </c>
       <c r="C29" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,7 +2163,7 @@
         <v>2.8322440087145972</v>
       </c>
       <c r="C30" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D30" t="s">
         <v>168</v>
@@ -2179,7 +2211,7 @@
         <v>0.8</v>
       </c>
       <c r="C34" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2190,96 +2222,107 @@
         <v>0.65</v>
       </c>
       <c r="C35" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B36">
         <v>0.3</v>
       </c>
       <c r="C36" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B37">
         <v>0.3</v>
       </c>
       <c r="C37" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <f>6.5/12</f>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <f>1/0.29</f>
+        <v>3.4482758620689657</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B41">
-        <v>0.25</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B42">
-        <v>0.25</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B43">
-        <v>0.1</v>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>262</v>
+      </c>
+      <c r="B44">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="193" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -2545,7 +2588,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2553,7 +2596,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -2564,7 +2607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -2687,7 +2730,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B7" s="11">
         <v>1</v>
@@ -2704,7 +2747,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B8" s="11">
         <v>1</v>
@@ -2718,7 +2761,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B9" s="11">
         <v>0.66</v>
@@ -2955,14 +2998,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -2984,7 +3027,7 @@
         <v>133</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3237,7 +3280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -3391,7 +3434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3418,7 +3461,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -3426,7 +3469,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -3434,7 +3477,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -3442,7 +3485,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -3450,7 +3493,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3458,7 +3501,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3469,12 +3512,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3499,49 +3542,49 @@
     </row>
     <row r="2" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B2" s="25">
-        <v>0.2382</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B3" s="18">
-        <v>0.1033</v>
+        <v>7.3099999999999998E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B4">
-        <v>0.34599999999999997</v>
+        <v>3.4599999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B5">
-        <v>0.29930000000000001</v>
+        <v>0.17469999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B6">
-        <v>4.0800000000000003E-2</v>
+        <v>8.3099999999999993E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B7">
         <v>0.02</v>
@@ -3549,7 +3592,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B8">
         <v>0.02</v>
@@ -3557,39 +3600,39 @@
     </row>
     <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B9" s="18">
-        <v>0.18540000000000001</v>
+        <v>0.4914</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B10">
-        <v>0.34599999999999997</v>
+        <v>1.0365</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B11">
-        <v>0.3634</v>
+        <v>0.84970000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B12">
-        <v>3.6999999999999998E-2</v>
+        <v>8.3099999999999993E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B13">
         <v>0.02</v>
@@ -3597,7 +3640,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B14">
         <v>0.02</v>
@@ -3605,39 +3648,39 @@
     </row>
     <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B15" s="18">
-        <v>0.18540000000000001</v>
+        <v>0.55620000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B16">
-        <v>0.50109999999999999</v>
+        <v>1.0365</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B17">
-        <v>0.3634</v>
+        <v>0.84970000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B18">
-        <v>5.5500000000000001E-2</v>
+        <v>8.3099999999999993E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B19">
         <v>0.02</v>
@@ -3645,7 +3688,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B20">
         <v>0.02</v>
@@ -3653,99 +3696,99 @@
     </row>
     <row r="21" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B21" s="18">
         <v>500</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B22" s="20">
-        <v>999</v>
+        <v>494</v>
       </c>
       <c r="C22" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B23" s="20">
-        <v>1033</v>
+        <v>494</v>
       </c>
       <c r="C23" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B24" s="20">
-        <v>1841</v>
+        <v>797</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B25" s="20">
-        <v>5243</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B26" s="20">
-        <v>7780</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B27" s="20">
-        <v>8376</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B28" s="20">
-        <v>7956</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B29" s="20">
-        <v>7353</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B30" s="20">
-        <v>0.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B31" s="20">
-        <v>0.6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3759,10 +3802,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,27 +3855,35 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
-        <v>1995</v>
+        <v>2005</v>
       </c>
       <c r="B6" s="11">
-        <v>100000</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
+        <v>2000</v>
+      </c>
+      <c r="B7" s="11">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>1995</v>
+      </c>
+      <c r="B8" s="11">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>1980</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B9" s="11">
         <v>25000</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
@@ -3917,14 +3968,6 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
     </row>
   </sheetData>
   <sortState ref="A1:B32">
@@ -4125,38 +4168,35 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="6" width="12.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -4174,7 +4214,7 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4190,7 +4230,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4253,8 +4293,8 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4280,23 +4320,35 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
+        <v>2014</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2010</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2008</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>2005</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B6" s="6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" s="3"/>
@@ -4315,7 +4367,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4380,99 +4432,83 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>267</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="I1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2009</v>
       </c>
-      <c r="B2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C2" t="s">
-        <v>266</v>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.114</v>
       </c>
       <c r="D2">
-        <v>0.114</v>
+        <f>C2*(1-0.154)</f>
+        <v>9.6444000000000002E-2</v>
       </c>
       <c r="E2">
-        <f>D2*(1-0.154)</f>
-        <v>9.6444000000000002E-2</v>
-      </c>
-      <c r="F2">
         <v>2190</v>
       </c>
+      <c r="F2" t="s">
+        <v>274</v>
+      </c>
       <c r="G2" t="s">
-        <v>268</v>
-      </c>
-      <c r="H2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2003</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <f>C3*(1-0.244)</f>
+        <v>8.0891999999999995E-3</v>
+      </c>
+      <c r="E3">
+        <v>1398</v>
+      </c>
+      <c r="F3" t="s">
         <v>276</v>
       </c>
-      <c r="C3" t="s">
-        <v>266</v>
-      </c>
-      <c r="D3">
-        <v>1.0699999999999999E-2</v>
-      </c>
-      <c r="E3">
-        <f>D3*(1-0.244)</f>
-        <v>8.0891999999999995E-3</v>
-      </c>
-      <c r="F3">
-        <v>1398</v>
-      </c>
       <c r="G3" t="s">
-        <v>277</v>
-      </c>
-      <c r="H3" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes and new analysis
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="80" windowWidth="20730" windowHeight="11760" tabRatio="923" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="80" windowWidth="20730" windowHeight="11760" tabRatio="923" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="270">
   <si>
     <t>Year</t>
   </si>
@@ -993,6 +993,15 @@
   </si>
   <si>
     <t>diagnosed_risk_reduction</t>
+  </si>
+  <si>
+    <t>c_NSP</t>
+  </si>
+  <si>
+    <t>c_OST</t>
+  </si>
+  <si>
+    <t>133 eurospeper year</t>
   </si>
 </sst>
 </file>
@@ -1517,8 +1526,8 @@
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1776,7 +1785,7 @@
         <v>166</v>
       </c>
       <c r="B21">
-        <v>5000</v>
+        <v>40000</v>
       </c>
       <c r="C21" t="s">
         <v>174</v>
@@ -1987,7 +1996,7 @@
         <v>253</v>
       </c>
       <c r="B39" s="32">
-        <v>0.25</v>
+        <v>100</v>
       </c>
       <c r="D39">
         <f>6.5/12</f>
@@ -1999,7 +2008,7 @@
         <v>255</v>
       </c>
       <c r="B40">
-        <v>0.25</v>
+        <v>100</v>
       </c>
       <c r="D40">
         <f>1/0.29</f>
@@ -2059,10 +2068,10 @@
   <sheetPr codeName="Sheet11">
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2330,7 +2339,7 @@
         <v>208</v>
       </c>
       <c r="B28">
-        <v>2100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -2349,12 +2358,31 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="31" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="13">
         <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="B32" s="20">
+        <v>155</v>
+      </c>
+      <c r="D32" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="B33">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>